<commit_message>
fixed: diff = buy - sell
</commit_message>
<xml_diff>
--- a/完成データ/時系列グループ別合計データ.xlsx
+++ b/完成データ/時系列グループ別合計データ.xlsx
@@ -447,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,13 +733,168 @@
         <v>161015.9</v>
       </c>
       <c r="G10" t="n">
-        <v>0.07188224572437753</v>
+        <v>0.07188224572437772</v>
       </c>
       <c r="H10" t="n">
         <v>8660.699999999999</v>
       </c>
       <c r="I10" t="n">
         <v>-0.09446686602120426</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>2020-08-24</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>10974.5</v>
+      </c>
+      <c r="C11" t="n">
+        <v>-0.2207990457459724</v>
+      </c>
+      <c r="D11" t="n">
+        <v>15507.3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-0.2064589420680692</v>
+      </c>
+      <c r="F11" t="n">
+        <v>109541.8</v>
+      </c>
+      <c r="G11" t="n">
+        <v>-0.3196833356208921</v>
+      </c>
+      <c r="H11" t="n">
+        <v>4700.299999999999</v>
+      </c>
+      <c r="I11" t="n">
+        <v>-0.4572840532520466</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>2020-08-25</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>19049.6</v>
+      </c>
+      <c r="C12" t="n">
+        <v>0.7358057314684039</v>
+      </c>
+      <c r="D12" t="n">
+        <v>28799.3</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.8571446995930949</v>
+      </c>
+      <c r="F12" t="n">
+        <v>167733.5</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.5312282617229221</v>
+      </c>
+      <c r="H12" t="n">
+        <v>12142.2</v>
+      </c>
+      <c r="I12" t="n">
+        <v>1.583281918175436</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="1" t="inlineStr">
+        <is>
+          <t>2020-08-26</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>11468.3</v>
+      </c>
+      <c r="C13" t="n">
+        <v>-0.3979768604065177</v>
+      </c>
+      <c r="D13" t="n">
+        <v>15837.7</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-0.4500664946717455</v>
+      </c>
+      <c r="F13" t="n">
+        <v>115022.1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>-0.3142568419546483</v>
+      </c>
+      <c r="H13" t="n">
+        <v>7992.799999999999</v>
+      </c>
+      <c r="I13" t="n">
+        <v>-0.3417337879461713</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="1" t="inlineStr">
+        <is>
+          <t>2020-08-27</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>9505.5</v>
+      </c>
+      <c r="C14" t="n">
+        <v>-0.1711500396745812</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12331.3</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.2213957834786618</v>
+      </c>
+      <c r="F14" t="n">
+        <v>101931.2</v>
+      </c>
+      <c r="G14" t="n">
+        <v>-0.1138120413381429</v>
+      </c>
+      <c r="H14" t="n">
+        <v>2607</v>
+      </c>
+      <c r="I14" t="n">
+        <v>-0.6738314483034731</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="1" t="inlineStr">
+        <is>
+          <t>2020-08-28</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>32544.6</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2.423765188575036</v>
+      </c>
+      <c r="D15" t="n">
+        <v>39411.8</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2.196078272363823</v>
+      </c>
+      <c r="F15" t="n">
+        <v>321223.4</v>
+      </c>
+      <c r="G15" t="n">
+        <v>2.151374652706924</v>
+      </c>
+      <c r="H15" t="n">
+        <v>16661.2</v>
+      </c>
+      <c r="I15" t="n">
+        <v>5.390947449175298</v>
       </c>
     </row>
   </sheetData>

</xml_diff>